<commit_message>
Added value sets for hearing laterality
</commit_message>
<xml_diff>
--- a/output/ValueSet-SPLASCHHearingObservationVS.xlsx
+++ b/output/ValueSet-SPLASCHHearingObservationVS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-24T23:37:25-04:00</t>
+    <t>2022-03-26T00:24:52-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>Need for and availability of a hearing aid [CMS Assessment]</t>
+  </si>
+  <si>
+    <t>67467-1</t>
+  </si>
+  <si>
+    <t>In which ear(s) do you have a hearing difficulty?</t>
+  </si>
+  <si>
+    <t>67242-8</t>
+  </si>
+  <si>
+    <t>Do you hear better in one ear than the other [PhenX]</t>
   </si>
   <si>
     <t/>
@@ -407,7 +419,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -462,15 +474,31 @@
         <v>37</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code cleanup. Added comments. No change to actual IG content
</commit_message>
<xml_diff>
--- a/output/ValueSet-SPLASCHHearingObservationVS.xlsx
+++ b/output/ValueSet-SPLASCHHearingObservationVS.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-26T00:24:52-04:00</t>
+    <t>2022-03-28T21:41:27-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -105,7 +105,7 @@
     <t>95744-9</t>
   </si>
   <si>
-    <t>Hearing.ability to hear during assessment period [CMS Assessment]</t>
+    <t>Hearing ability to hear during assessment period [CMS Assessment]</t>
   </si>
   <si>
     <t>54599-6</t>

</xml_diff>

<commit_message>
added answer lists for new Hearing questions
</commit_message>
<xml_diff>
--- a/output/ValueSet-SPLASCHHearingObservationVS.xlsx
+++ b/output/ValueSet-SPLASCHHearingObservationVS.xlsx
@@ -9,12 +9,13 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Include from LOINC" r:id="rId4" sheetId="2"/>
     <sheet name="Include ValueSets" r:id="rId5" sheetId="3"/>
+    <sheet name="Include ValueSets 2" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Property</t>
   </si>
@@ -58,7 +59,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-15T08:42:50-04:00</t>
+    <t>2022-04-15T09:25:37-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -152,6 +153,9 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/pacio-splasch/ValueSet/SPLASCHPureToneThresholdAudiometryPanel</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/pacio-splasch/ValueSet/SPLASCHDiagnosticAudiologyResultsPanel</t>
   </si>
 </sst>
 </file>
@@ -538,4 +542,31 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="30.703125" customWidth="true"/>
+    <col min="2" max="2" width="50.703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix build errors by moving hearing response codes from value sets to code systems (similar to previous commits for other profiles)
</commit_message>
<xml_diff>
--- a/output/ValueSet-SPLASCHHearingObservationVS.xlsx
+++ b/output/ValueSet-SPLASCHHearingObservationVS.xlsx
@@ -8,14 +8,14 @@
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Include from LOINC" r:id="rId4" sheetId="2"/>
-    <sheet name="Include ValueSets" r:id="rId5" sheetId="3"/>
-    <sheet name="Include ValueSets 2" r:id="rId6" sheetId="4"/>
+    <sheet name="Include from Pure tone thresh" r:id="rId5" sheetId="3"/>
+    <sheet name="Include from Diagnostic Audio" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Property</t>
   </si>
@@ -59,7 +59,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-05-03T12:45:05-04:00</t>
+    <t>2022-05-03T15:05:17-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -149,13 +149,16 @@
     <t>http://loinc.org</t>
   </si>
   <si>
-    <t>ValueSet URL</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/pacio-splasch/ValueSet/SPLASCHPureToneThresholdAudiometryPanel</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/pacio-splasch/ValueSet/SPLASCHDiagnosticAudiologyResultsPanel</t>
+    <t>Codes</t>
+  </si>
+  <si>
+    <t>All codes</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/pacio-splasch/CodeSystem/SPLASCHPureToneThresholdAudiometryPanelCS</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/pacio-splasch/CodeSystem/SPLASCHDiagnosticAudiologyResultsPanelCS</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -539,6 +542,22 @@
         <v>45</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -546,7 +565,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -563,7 +582,23 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>